<commit_message>
Envelope breakage has been done
</commit_message>
<xml_diff>
--- a/wwwroot/reports/DuplicateTool 79.xlsx
+++ b/wwwroot/reports/DuplicateTool 79.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="285">
   <si>
     <t>Id</t>
   </si>
@@ -59,7 +59,7 @@
     <t>2201</t>
   </si>
   <si>
-    <t>173</t>
+    <t>180</t>
   </si>
   <si>
     <t>2216</t>
@@ -86,471 +86,465 @@
     <t xml:space="preserve">LLB - YEARLY  (3 YEAR)</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>106001</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>B.Ed. ( YEARLY)</t>
+  </si>
+  <si>
+    <t>B.ED (YEARLY)</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>BED-201</t>
+  </si>
+  <si>
+    <t>KNOWLEDGE &amp; CURRICULUM</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Diploma in Yoga Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yoga Education</t>
+  </si>
+  <si>
+    <t>2205</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>1264</t>
+  </si>
+  <si>
+    <t>324101</t>
+  </si>
+  <si>
+    <t>YOGA PARICHAYA</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
-    <t>106001</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>B.Ed. ( YEARLY)</t>
-  </si>
-  <si>
-    <t>B.ED (YEARLY)</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>B.Sc.FORESTRY (Yearly)</t>
+  </si>
+  <si>
+    <t>B.SC.FORESTRY (YEARLY)</t>
+  </si>
+  <si>
+    <t>2225</t>
+  </si>
+  <si>
+    <t>91501</t>
+  </si>
+  <si>
+    <t>ELEMENTARY BIOCHEMISTRY AND NUTRITION</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2208</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>2212</t>
+  </si>
+  <si>
+    <t>PGDCP</t>
+  </si>
+  <si>
+    <t>1259</t>
+  </si>
+  <si>
+    <t>838101</t>
+  </si>
+  <si>
+    <t>COMPUTER ORG. &amp; INFORMATION TECH.</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3301</t>
+  </si>
+  <si>
+    <t>03:00 PM TO 05:00 PM</t>
+  </si>
+  <si>
+    <t>101001</t>
+  </si>
+  <si>
+    <t>CONTRACT I</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>3309</t>
+  </si>
+  <si>
+    <t>107001</t>
+  </si>
+  <si>
+    <t>LAND LAWS</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>BED-201</t>
-  </si>
-  <si>
-    <t>KNOWLEDGE &amp; CURRICULUM</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Diploma in Yoga Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yoga Education</t>
-  </si>
-  <si>
-    <t>2205</t>
+    <t>2217</t>
+  </si>
+  <si>
+    <t>45861</t>
+  </si>
+  <si>
+    <t>103002</t>
+  </si>
+  <si>
+    <t>CRIMINAL PROCEDURE CODE, CHILD CARE AND PROTECTION ACT,2000</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>106002</t>
+  </si>
+  <si>
+    <t>CRIMINAL PROCEDURE CODE, CHILD CARE AND PROTECTION ACT, 2000</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>2202</t>
+  </si>
+  <si>
+    <t>BED-202</t>
+  </si>
+  <si>
+    <t>ASSESSMENT FOR LEARNING</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>1265</t>
+  </si>
+  <si>
+    <t>324102</t>
+  </si>
+  <si>
+    <t>PATANJALI YOGA SUTRA</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>2227</t>
+  </si>
+  <si>
+    <t>91503</t>
+  </si>
+  <si>
+    <t>FUNDAMENTALS OF GENETIC AND INTRODUCTORY PLANT BREEDING AND ELEMENTS OF APPLIED STATISTICS</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1260</t>
+  </si>
+  <si>
+    <t>838102</t>
+  </si>
+  <si>
+    <t>OPERATING SYSTEM</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>3302</t>
+  </si>
+  <si>
+    <t>101002</t>
+  </si>
+  <si>
+    <t>ARBITRATION CONCILIATION AND ALTERNATE DISPUTE RESOLUTION SYSTEM</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>3310</t>
+  </si>
+  <si>
+    <t>107002</t>
+  </si>
+  <si>
+    <t>HUMAN RIGHTS AND INTERNATIONAL LAWS</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>2218</t>
+  </si>
+  <si>
+    <t>45863</t>
+  </si>
+  <si>
+    <t>103003</t>
+  </si>
+  <si>
+    <t>PROPERTY-LAW INCLUDING TRANSFER OF PROPERTY ACT AND EASEMENT ACT.</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>106003</t>
+  </si>
+  <si>
+    <t>PROPERTY LAW INCLUDING TRANSFER OF PROPERTY ACT</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>2203</t>
+  </si>
+  <si>
+    <t>BED-203</t>
+  </si>
+  <si>
+    <t>CREATING AN INCLUSIVE SCHOOL</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>1266</t>
+  </si>
+  <si>
+    <t>324103</t>
+  </si>
+  <si>
+    <t>YOGA AND MENTAL HEALTH</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>2228</t>
+  </si>
+  <si>
+    <t>91504</t>
+  </si>
+  <si>
+    <t>FOREST MENSURATION AND USE OF REMOTE SENSING TECHNIQUES AND PRACTICAL FIELD FORESTRY</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>1264</t>
-  </si>
-  <si>
-    <t>324101</t>
-  </si>
-  <si>
-    <t>YOGA PARICHAYA</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>B.Sc.FORESTRY (Yearly)</t>
-  </si>
-  <si>
-    <t>B.SC.FORESTRY (YEARLY)</t>
-  </si>
-  <si>
-    <t>2225</t>
-  </si>
-  <si>
-    <t>91501</t>
-  </si>
-  <si>
-    <t>ELEMENTARY BIOCHEMISTRY AND NUTRITION</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>2208</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>2212</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>PGDCP</t>
-  </si>
-  <si>
-    <t>1259</t>
-  </si>
-  <si>
-    <t>838101</t>
-  </si>
-  <si>
-    <t>COMPUTER ORG. &amp; INFORMATION TECH.</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>3301</t>
-  </si>
-  <si>
-    <t>03:00 PM TO 05:00 PM</t>
-  </si>
-  <si>
-    <t>101001</t>
-  </si>
-  <si>
-    <t>CONTRACT I</t>
-  </si>
-  <si>
-    <t>12</t>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>1261</t>
+  </si>
+  <si>
+    <t>838103</t>
+  </si>
+  <si>
+    <t>DATS STRUCTURE IN C</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>3303</t>
+  </si>
+  <si>
+    <t>101003</t>
+  </si>
+  <si>
+    <t>TORTS AND CONSUMER PROTECTION LAWS</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>3311</t>
+  </si>
+  <si>
+    <t>107003</t>
+  </si>
+  <si>
+    <t>ADMINISTRATIVE LAW</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>2219</t>
+  </si>
+  <si>
+    <t>45866</t>
+  </si>
+  <si>
+    <t>103004</t>
+  </si>
+  <si>
+    <t>LAW OF EVIDENCE</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>106004</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>2204</t>
+  </si>
+  <si>
+    <t>BED-204</t>
+  </si>
+  <si>
+    <t>YOGA EDUCATION</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>1267</t>
+  </si>
+  <si>
+    <t>324104</t>
+  </si>
+  <si>
+    <t>ANATOMY &amp; PHYSIOLOGY</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>2230</t>
+  </si>
+  <si>
+    <t>91506</t>
+  </si>
+  <si>
+    <t>FRUIT GROWING</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>1262</t>
+  </si>
+  <si>
+    <t>838104</t>
+  </si>
+  <si>
+    <t>DBMS AND FINANCIAL ACCOUNTING</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>3304</t>
+  </si>
+  <si>
+    <t>101004</t>
+  </si>
+  <si>
+    <t>FAMILY LAW I HINDU LAW</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
-    <t>3309</t>
-  </si>
-  <si>
-    <t>107001</t>
-  </si>
-  <si>
-    <t>LAND LAWS</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>174</t>
-  </si>
-  <si>
-    <t>2217</t>
-  </si>
-  <si>
-    <t>45861</t>
-  </si>
-  <si>
-    <t>103002</t>
-  </si>
-  <si>
-    <t>CRIMINAL PROCEDURE CODE, CHILD CARE AND PROTECTION ACT,2000</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>106002</t>
-  </si>
-  <si>
-    <t>CRIMINAL PROCEDURE CODE, CHILD CARE AND PROTECTION ACT, 2000</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>2202</t>
-  </si>
-  <si>
-    <t>BED-202</t>
-  </si>
-  <si>
-    <t>ASSESSMENT FOR LEARNING</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>1265</t>
-  </si>
-  <si>
-    <t>324102</t>
-  </si>
-  <si>
-    <t>PATANJALI YOGA SUTRA</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>2227</t>
-  </si>
-  <si>
-    <t>91503</t>
-  </si>
-  <si>
-    <t>FUNDAMENTALS OF GENETIC AND INTRODUCTORY PLANT BREEDING AND ELEMENTS OF APPLIED STATISTICS</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>1260</t>
-  </si>
-  <si>
-    <t>838102</t>
-  </si>
-  <si>
-    <t>OPERATING SYSTEM</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>3302</t>
-  </si>
-  <si>
-    <t>101002</t>
-  </si>
-  <si>
-    <t>ARBITRATION CONCILIATION AND ALTERNATE DISPUTE RESOLUTION SYSTEM</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>3310</t>
-  </si>
-  <si>
-    <t>107002</t>
-  </si>
-  <si>
-    <t>HUMAN RIGHTS AND INTERNATIONAL LAWS</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>171</t>
-  </si>
-  <si>
-    <t>2218</t>
-  </si>
-  <si>
-    <t>45863</t>
-  </si>
-  <si>
-    <t>103003</t>
-  </si>
-  <si>
-    <t>PROPERTY-LAW INCLUDING TRANSFER OF PROPERTY ACT AND EASEMENT ACT.</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>106003</t>
-  </si>
-  <si>
-    <t>PROPERTY LAW INCLUDING TRANSFER OF PROPERTY ACT</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>2203</t>
-  </si>
-  <si>
-    <t>BED-203</t>
-  </si>
-  <si>
-    <t>CREATING AN INCLUSIVE SCHOOL</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>1266</t>
-  </si>
-  <si>
-    <t>324103</t>
-  </si>
-  <si>
-    <t>YOGA AND MENTAL HEALTH</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>2228</t>
-  </si>
-  <si>
-    <t>91504</t>
-  </si>
-  <si>
-    <t>FOREST MENSURATION AND USE OF REMOTE SENSING TECHNIQUES AND PRACTICAL FIELD FORESTRY</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>1261</t>
-  </si>
-  <si>
-    <t>838103</t>
-  </si>
-  <si>
-    <t>DATS STRUCTURE IN C</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>3303</t>
-  </si>
-  <si>
-    <t>101003</t>
-  </si>
-  <si>
-    <t>TORTS AND CONSUMER PROTECTION LAWS</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>3311</t>
-  </si>
-  <si>
-    <t>107003</t>
-  </si>
-  <si>
-    <t>ADMINISTRATIVE LAW</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>2219</t>
-  </si>
-  <si>
-    <t>45866</t>
-  </si>
-  <si>
-    <t>103004</t>
-  </si>
-  <si>
-    <t>LAW OF EVIDENCE</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>106004</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>2204</t>
-  </si>
-  <si>
-    <t>BED-204</t>
-  </si>
-  <si>
-    <t>YOGA EDUCATION</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>1267</t>
-  </si>
-  <si>
-    <t>324104</t>
-  </si>
-  <si>
-    <t>ANATOMY &amp; PHYSIOLOGY</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>2230</t>
-  </si>
-  <si>
-    <t>91506</t>
-  </si>
-  <si>
-    <t>FRUIT GROWING</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>1262</t>
-  </si>
-  <si>
-    <t>838104</t>
-  </si>
-  <si>
-    <t>DBMS AND FINANCIAL ACCOUNTING</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>3304</t>
-  </si>
-  <si>
-    <t>101004</t>
-  </si>
-  <si>
-    <t>FAMILY LAW I HINDU LAW</t>
-  </si>
-  <si>
     <t>3312</t>
   </si>
   <si>
@@ -567,9 +561,6 @@
   </si>
   <si>
     <t>61</t>
-  </si>
-  <si>
-    <t>172</t>
   </si>
   <si>
     <t>2220</t>
@@ -903,7 +894,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8B0000"/>
+        <fgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1129,7 +1120,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>12</v>
@@ -1144,7 +1135,7 @@
         <v>35</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>14</v>
@@ -1164,25 +1155,25 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>17</v>
@@ -1191,15 +1182,15 @@
         <v>18</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>12</v>
@@ -1211,10 +1202,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>16</v>
@@ -1234,7 +1225,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>12</v>
@@ -1246,10 +1237,10 @@
         <v>28</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>14</v>
@@ -1269,7 +1260,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>12</v>
@@ -1281,10 +1272,10 @@
         <v>28</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>14</v>
@@ -1304,7 +1295,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>12</v>
@@ -1316,10 +1307,10 @@
         <v>52</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>53</v>
@@ -1354,27 +1345,27 @@
         <v>14</v>
       </c>
       <c r="F12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="K12" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>12</v>
@@ -1389,27 +1380,27 @@
         <v>14</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>12</v>
@@ -1427,24 +1418,24 @@
         <v>24</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>12</v>
@@ -1456,30 +1447,30 @@
         <v>13</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="K15" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>12</v>
@@ -1491,30 +1482,30 @@
         <v>23</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>12</v>
@@ -1529,27 +1520,27 @@
         <v>14</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="I17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="0" t="s">
+      <c r="K17" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
@@ -1564,27 +1555,27 @@
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="I18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>12</v>
@@ -1605,7 +1596,7 @@
         <v>79</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>18</v>
@@ -1634,27 +1625,27 @@
         <v>35</v>
       </c>
       <c r="F20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="H20" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="0" t="s">
+      <c r="K20" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="K20" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>12</v>
@@ -1669,13 +1660,13 @@
         <v>35</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>79</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I21" s="0" t="s">
         <v>18</v>
@@ -1689,42 +1680,42 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G22" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K22" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>12</v>
@@ -1736,30 +1727,30 @@
         <v>13</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G23" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="I23" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="0" t="s">
+      <c r="K23" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>12</v>
@@ -1771,16 +1762,16 @@
         <v>28</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>79</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I24" s="0" t="s">
         <v>18</v>
@@ -1794,7 +1785,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>12</v>
@@ -1806,16 +1797,16 @@
         <v>28</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>79</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I25" s="0" t="s">
         <v>18</v>
@@ -1829,7 +1820,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>12</v>
@@ -1841,30 +1832,30 @@
         <v>52</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G26" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="K26" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="K26" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>12</v>
@@ -1879,27 +1870,27 @@
         <v>14</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="G27" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="K27" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J27" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>12</v>
@@ -1914,27 +1905,27 @@
         <v>14</v>
       </c>
       <c r="F28" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="K28" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>12</v>
@@ -1949,27 +1940,27 @@
         <v>35</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>12</v>
@@ -1981,30 +1972,30 @@
         <v>13</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G30" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="H30" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J30" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K30" s="0" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>12</v>
@@ -2016,30 +2007,30 @@
         <v>23</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>29</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>12</v>
@@ -2054,27 +2045,27 @@
         <v>14</v>
       </c>
       <c r="F32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="K32" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>12</v>
@@ -2089,27 +2080,27 @@
         <v>14</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="K33" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>12</v>
@@ -2124,27 +2115,27 @@
         <v>14</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>12</v>
@@ -2159,27 +2150,27 @@
         <v>35</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>12</v>
@@ -2197,59 +2188,59 @@
         <v>24</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>12</v>
@@ -2261,30 +2252,30 @@
         <v>13</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>12</v>
@@ -2296,30 +2287,30 @@
         <v>28</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>12</v>
@@ -2331,30 +2322,30 @@
         <v>28</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>133</v>
+        <v>36</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>12</v>
@@ -2366,30 +2357,30 @@
         <v>52</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>12</v>
@@ -2404,27 +2395,27 @@
         <v>14</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>12</v>
@@ -2439,27 +2430,27 @@
         <v>14</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>12</v>
@@ -2474,27 +2465,27 @@
         <v>35</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>12</v>
@@ -2506,30 +2497,30 @@
         <v>13</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>12</v>
@@ -2541,30 +2532,30 @@
         <v>23</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>12</v>
@@ -2579,27 +2570,27 @@
         <v>14</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>111</v>
+        <v>15</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>12</v>
@@ -2614,27 +2605,27 @@
         <v>14</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J48" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="K48" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>12</v>
@@ -2649,27 +2640,27 @@
         <v>14</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>12</v>
@@ -2684,27 +2675,27 @@
         <v>35</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>12</v>
@@ -2719,62 +2710,62 @@
         <v>35</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>12</v>
@@ -2786,30 +2777,30 @@
         <v>13</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>12</v>
@@ -2821,30 +2812,30 @@
         <v>28</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>12</v>
@@ -2856,30 +2847,30 @@
         <v>28</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>12</v>
@@ -2891,30 +2882,30 @@
         <v>52</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I56" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>12</v>
@@ -2929,27 +2920,27 @@
         <v>14</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>12</v>
@@ -2964,27 +2955,27 @@
         <v>14</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="G58" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="K58" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="H58" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="I58" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J58" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="K58" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>12</v>
@@ -2999,27 +2990,27 @@
         <v>35</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G59" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="K59" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="H59" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="I59" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J59" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="K59" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>12</v>
@@ -3031,30 +3022,30 @@
         <v>13</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J60" s="0" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K60" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>12</v>
@@ -3066,30 +3057,30 @@
         <v>23</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="G61" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="K61" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="K61" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>12</v>
@@ -3104,27 +3095,27 @@
         <v>14</v>
       </c>
       <c r="F62" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="G62" s="0" t="s">
+      <c r="K62" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="H62" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="I62" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J62" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="K62" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>12</v>
@@ -3139,27 +3130,27 @@
         <v>14</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K63" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>12</v>
@@ -3174,62 +3165,62 @@
         <v>35</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G64" s="0" t="s">
         <v>35</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I65" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J65" s="0" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="K65" s="0" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>12</v>
@@ -3241,30 +3232,30 @@
         <v>13</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G66" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="K66" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="H66" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="I66" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J66" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="K66" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>12</v>
@@ -3276,30 +3267,30 @@
         <v>52</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I67" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>12</v>
@@ -3314,27 +3305,27 @@
         <v>14</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K68" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>12</v>
@@ -3349,27 +3340,27 @@
         <v>14</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>170</v>
+        <v>62</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K69" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>12</v>
@@ -3384,27 +3375,27 @@
         <v>35</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J70" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K70" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>12</v>
@@ -3416,30 +3407,30 @@
         <v>13</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K71" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>12</v>
@@ -3451,30 +3442,30 @@
         <v>23</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I72" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J72" s="0" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K72" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>12</v>
@@ -3489,27 +3480,27 @@
         <v>14</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="G73" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="K73" s="0" t="s">
         <v>216</v>
-      </c>
-      <c r="H73" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="I73" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="K73" s="0" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>12</v>
@@ -3524,27 +3515,27 @@
         <v>14</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>12</v>
@@ -3559,62 +3550,62 @@
         <v>14</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I75" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K75" s="0" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E76" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I76" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K76" s="0" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>12</v>
@@ -3626,30 +3617,30 @@
         <v>13</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G77" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="K77" s="0" t="s">
         <v>216</v>
-      </c>
-      <c r="H77" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="I77" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J77" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="K77" s="0" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>12</v>
@@ -3664,27 +3655,27 @@
         <v>14</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K78" s="0" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>12</v>
@@ -3699,22 +3690,22 @@
         <v>14</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J79" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K79" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80">
@@ -3734,27 +3725,27 @@
         <v>35</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I80" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K80" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>12</v>
@@ -3766,30 +3757,30 @@
         <v>13</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I81" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="K81" s="0" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>12</v>
@@ -3801,30 +3792,30 @@
         <v>23</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I82" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="K82" s="0" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>12</v>
@@ -3842,24 +3833,24 @@
         <v>15</v>
       </c>
       <c r="G83" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="K83" s="0" t="s">
         <v>243</v>
-      </c>
-      <c r="H83" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="I83" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J83" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="K83" s="0" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>12</v>
@@ -3877,24 +3868,24 @@
         <v>24</v>
       </c>
       <c r="G84" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="K84" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="H84" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="K84" s="2" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>12</v>
@@ -3906,30 +3897,30 @@
         <v>13</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F85" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G85" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J85" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="K85" s="0" t="s">
         <v>243</v>
-      </c>
-      <c r="H85" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="I85" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J85" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="K85" s="0" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>12</v>
@@ -3944,27 +3935,27 @@
         <v>14</v>
       </c>
       <c r="F86" s="0" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I86" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J86" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K86" s="0" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>12</v>
@@ -3979,27 +3970,27 @@
         <v>14</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I87" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J87" s="0" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K87" s="0" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>12</v>
@@ -4014,27 +4005,27 @@
         <v>35</v>
       </c>
       <c r="F88" s="0" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I88" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K88" s="0" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>12</v>
@@ -4046,30 +4037,30 @@
         <v>13</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I89" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J89" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K89" s="0" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>12</v>
@@ -4081,30 +4072,30 @@
         <v>23</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F90" s="0" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="I90" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J90" s="0" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="K90" s="0" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>12</v>
@@ -4119,27 +4110,27 @@
         <v>14</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="G91" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H91" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J91" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="K91" s="0" t="s">
         <v>262</v>
-      </c>
-      <c r="H91" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="I91" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J91" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="K91" s="0" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>12</v>
@@ -4154,27 +4145,27 @@
         <v>14</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G92" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="K92" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="H92" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="K92" s="2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>12</v>
@@ -4189,27 +4180,27 @@
         <v>14</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I93" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="K93" s="0" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>12</v>
@@ -4221,30 +4212,30 @@
         <v>13</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G94" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H94" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I94" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J94" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="K94" s="0" t="s">
         <v>262</v>
-      </c>
-      <c r="H94" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="I94" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J94" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="K94" s="0" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>12</v>
@@ -4259,27 +4250,27 @@
         <v>14</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H95" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I95" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K95" s="0" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>12</v>
@@ -4294,27 +4285,27 @@
         <v>14</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>165</v>
+        <v>62</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H96" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I96" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K96" s="0" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>12</v>
@@ -4332,24 +4323,24 @@
         <v>24</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H97" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I97" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K97" s="0" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>12</v>
@@ -4361,30 +4352,30 @@
         <v>13</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F98" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H98" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I98" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="K98" s="0" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>12</v>
@@ -4396,30 +4387,30 @@
         <v>23</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F99" s="0" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H99" s="0" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I99" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K99" s="0" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>12</v>
@@ -4434,22 +4425,22 @@
         <v>14</v>
       </c>
       <c r="F100" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G100" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="H100" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="I100" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J100" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="K100" s="0" t="s">
         <v>284</v>
-      </c>
-      <c r="H100" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="I100" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J100" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="K100" s="0" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>